<commit_message>
Added GOOG, NFLX, FICO, ADSK, META, TYL, ANET, AVGO, AMAT
</commit_message>
<xml_diff>
--- a/Cybersecurity/Fortinet.xlsx
+++ b/Cybersecurity/Fortinet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Technology/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Cybersecurity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFBD6A9-5930-7849-A258-D92BDB901E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D22710-BAA6-8B43-B4DB-EF2550B3629E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30220" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -977,6 +977,12 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -994,12 +1000,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2475,8 +2475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R67" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="T96" sqref="T96"/>
@@ -3755,7 +3755,7 @@
       <c r="Q19" s="10">
         <v>720200000</v>
       </c>
-      <c r="W19" s="68">
+      <c r="W19" s="62">
         <f>Q40-Q56-Q61</f>
         <v>1563300000</v>
       </c>
@@ -7210,10 +7210,10 @@
       <c r="Q83" s="1">
         <v>-19400000</v>
       </c>
-      <c r="X83" s="64" t="s">
+      <c r="X83" s="66" t="s">
         <v>123</v>
       </c>
-      <c r="Y83" s="65"/>
+      <c r="Y83" s="67"/>
     </row>
     <row r="84" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
@@ -7267,10 +7267,10 @@
       <c r="Q84" s="1">
         <v>-13100000</v>
       </c>
-      <c r="X84" s="66" t="s">
+      <c r="X84" s="68" t="s">
         <v>124</v>
       </c>
-      <c r="Y84" s="67"/>
+      <c r="Y84" s="69"/>
     </row>
     <row r="85" spans="1:25" ht="20" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -7818,10 +7818,10 @@
         <v>1300000</v>
       </c>
       <c r="Q93" s="1"/>
-      <c r="X93" s="66" t="s">
+      <c r="X93" s="68" t="s">
         <v>131</v>
       </c>
-      <c r="Y93" s="67"/>
+      <c r="Y93" s="69"/>
     </row>
     <row r="94" spans="1:25" ht="20" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
@@ -8112,10 +8112,10 @@
       <c r="Q98" s="35">
         <v>0</v>
       </c>
-      <c r="X98" s="66" t="s">
+      <c r="X98" s="68" t="s">
         <v>135</v>
       </c>
-      <c r="Y98" s="67"/>
+      <c r="Y98" s="69"/>
     </row>
     <row r="99" spans="1:25" ht="20" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
@@ -8468,10 +8468,10 @@
       <c r="Q104" s="11">
         <v>1319100000</v>
       </c>
-      <c r="X104" s="66" t="s">
+      <c r="X104" s="68" t="s">
         <v>140</v>
       </c>
-      <c r="Y104" s="67"/>
+      <c r="Y104" s="69"/>
     </row>
     <row r="105" spans="1:25" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
@@ -8704,10 +8704,10 @@
       </c>
     </row>
     <row r="109" spans="1:25" ht="19" x14ac:dyDescent="0.25">
-      <c r="R109" s="62" t="s">
+      <c r="R109" s="64" t="s">
         <v>147</v>
       </c>
-      <c r="S109" s="63"/>
+      <c r="S109" s="65"/>
     </row>
     <row r="110" spans="1:25" ht="20" x14ac:dyDescent="0.25">
       <c r="R110" s="47" t="s">
@@ -8749,7 +8749,7 @@
       <c r="R114" s="47" t="s">
         <v>151</v>
       </c>
-      <c r="S114" s="69">
+      <c r="S114" s="63">
         <f>Q34*(1+(5*W16))</f>
         <v>791545127.5039233</v>
       </c>

</xml_diff>